<commit_message>
Affichage nom/projet/choix dans main
</commit_message>
<xml_diff>
--- a/sujets choisis test.xlsx
+++ b/sujets choisis test.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robin\OneDrive\Documents\Projet IESE4 - Allocation de ressources\AllocationDeRessource\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{399A0977-F2B6-4F5E-915A-4B9E964EDBFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9E4F6F4-F470-4719-9C9C-1836EF76B5E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -501,8 +501,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="67" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="67" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="P27" sqref="P27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -574,11 +574,9 @@
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4">
-        <v>1</v>
-      </c>
+      <c r="B2" s="4"/>
       <c r="C2" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -587,67 +585,73 @@
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
+      <c r="K2" s="4">
+        <v>2</v>
+      </c>
       <c r="L2" s="4"/>
       <c r="M2" s="4"/>
       <c r="N2" s="4"/>
       <c r="O2" s="4"/>
       <c r="P2" s="4"/>
-      <c r="Q2" s="4"/>
+      <c r="Q2" s="4">
+        <v>3</v>
+      </c>
       <c r="R2" s="4"/>
       <c r="S2" s="4"/>
       <c r="T2">
-        <f>SUM(B2:S2)</f>
-        <v>3</v>
+        <f t="shared" ref="T2:T37" si="0">SUM(B2:S2)</f>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:20" ht="18" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="4">
-        <v>1</v>
-      </c>
-      <c r="C3" s="4">
-        <v>2</v>
-      </c>
-      <c r="D3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4">
+        <v>2</v>
+      </c>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
+      <c r="H3" s="4">
+        <v>3</v>
+      </c>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
       <c r="L3" s="4"/>
       <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
+      <c r="N3" s="4">
+        <v>1</v>
+      </c>
       <c r="O3" s="4"/>
       <c r="P3" s="4"/>
       <c r="Q3" s="4"/>
       <c r="R3" s="4"/>
       <c r="S3" s="4"/>
       <c r="T3">
-        <f>SUM(B3:S3)</f>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:20" ht="18" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4">
-        <v>1</v>
-      </c>
-      <c r="D4" s="4">
-        <v>2</v>
-      </c>
+      <c r="B4" s="4">
+        <v>1</v>
+      </c>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
+      <c r="I4" s="4">
+        <v>3</v>
+      </c>
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
       <c r="L4" s="4"/>
@@ -657,10 +661,12 @@
       <c r="P4" s="4"/>
       <c r="Q4" s="4"/>
       <c r="R4" s="4"/>
-      <c r="S4" s="4"/>
+      <c r="S4" s="4">
+        <v>2</v>
+      </c>
       <c r="T4">
-        <f>SUM(B4:S4)</f>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:20" ht="18" x14ac:dyDescent="0.3">
@@ -668,30 +674,32 @@
         <v>4</v>
       </c>
       <c r="B5" s="4"/>
-      <c r="C5" s="4">
-        <v>1</v>
-      </c>
-      <c r="D5" s="4">
-        <v>2</v>
-      </c>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
+      <c r="I5" s="4">
+        <v>2</v>
+      </c>
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
+      <c r="L5" s="4">
+        <v>3</v>
+      </c>
       <c r="M5" s="4"/>
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
       <c r="P5" s="4"/>
-      <c r="Q5" s="4"/>
+      <c r="Q5" s="4">
+        <v>1</v>
+      </c>
       <c r="R5" s="4"/>
       <c r="S5" s="4"/>
       <c r="T5">
-        <f>SUM(B5:S5)</f>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:20" ht="18" x14ac:dyDescent="0.3">
@@ -703,26 +711,28 @@
       <c r="D6" s="4">
         <v>1</v>
       </c>
-      <c r="E6" s="4">
-        <v>2</v>
-      </c>
+      <c r="E6" s="4"/>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
+      <c r="K6" s="4">
+        <v>3</v>
+      </c>
       <c r="L6" s="4"/>
       <c r="M6" s="4"/>
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
-      <c r="P6" s="4"/>
+      <c r="P6" s="4">
+        <v>2</v>
+      </c>
       <c r="Q6" s="4"/>
       <c r="R6" s="4"/>
       <c r="S6" s="4"/>
       <c r="T6">
-        <f>SUM(B6:S6)</f>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:20" ht="18" x14ac:dyDescent="0.3">
@@ -731,15 +741,17 @@
       </c>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
-      <c r="D7" s="4">
-        <v>1</v>
-      </c>
+      <c r="D7" s="4"/>
       <c r="E7" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
+      <c r="G7" s="4">
+        <v>2</v>
+      </c>
+      <c r="H7" s="4">
+        <v>1</v>
+      </c>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
@@ -752,8 +764,8 @@
       <c r="R7" s="4"/>
       <c r="S7" s="4"/>
       <c r="T7">
-        <f>SUM(B7:S7)</f>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:20" ht="18" x14ac:dyDescent="0.3">
@@ -762,17 +774,19 @@
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4">
-        <v>1</v>
-      </c>
-      <c r="F8" s="4">
-        <v>2</v>
-      </c>
+      <c r="D8" s="4">
+        <v>2</v>
+      </c>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
       <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
+      <c r="H8" s="4">
+        <v>3</v>
+      </c>
       <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
+      <c r="J8" s="4">
+        <v>1</v>
+      </c>
       <c r="K8" s="4"/>
       <c r="L8" s="4"/>
       <c r="M8" s="4"/>
@@ -783,8 +797,8 @@
       <c r="R8" s="4"/>
       <c r="S8" s="4"/>
       <c r="T8">
-        <f>SUM(B8:S8)</f>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:20" ht="18" x14ac:dyDescent="0.3">
@@ -794,44 +808,44 @@
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
-      <c r="E9" s="4">
-        <v>1</v>
-      </c>
+      <c r="E9" s="4"/>
       <c r="F9" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
+      <c r="K9" s="4">
+        <v>2</v>
+      </c>
       <c r="L9" s="4"/>
       <c r="M9" s="4"/>
       <c r="N9" s="4"/>
-      <c r="O9" s="4"/>
+      <c r="O9" s="4">
+        <v>3</v>
+      </c>
       <c r="P9" s="4"/>
       <c r="Q9" s="4"/>
       <c r="R9" s="4"/>
       <c r="S9" s="4"/>
       <c r="T9">
-        <f>SUM(B9:S9)</f>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:20" ht="18" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="4"/>
+      <c r="B10" s="4">
+        <v>2</v>
+      </c>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
-      <c r="F10" s="4">
-        <v>1</v>
-      </c>
-      <c r="G10" s="4">
-        <v>2</v>
-      </c>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
@@ -840,13 +854,17 @@
       <c r="M10" s="4"/>
       <c r="N10" s="4"/>
       <c r="O10" s="4"/>
-      <c r="P10" s="4"/>
+      <c r="P10" s="4">
+        <v>3</v>
+      </c>
       <c r="Q10" s="4"/>
       <c r="R10" s="4"/>
-      <c r="S10" s="4"/>
+      <c r="S10" s="4">
+        <v>1</v>
+      </c>
       <c r="T10">
-        <f>SUM(B10:S10)</f>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:20" ht="18" x14ac:dyDescent="0.3">
@@ -857,12 +875,8 @@
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
-      <c r="F11" s="4">
-        <v>1</v>
-      </c>
-      <c r="G11" s="4">
-        <v>2</v>
-      </c>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
@@ -870,14 +884,20 @@
       <c r="L11" s="4"/>
       <c r="M11" s="4"/>
       <c r="N11" s="4"/>
-      <c r="O11" s="4"/>
-      <c r="P11" s="4"/>
+      <c r="O11" s="4">
+        <v>3</v>
+      </c>
+      <c r="P11" s="4">
+        <v>2</v>
+      </c>
       <c r="Q11" s="4"/>
-      <c r="R11" s="4"/>
+      <c r="R11" s="4">
+        <v>1</v>
+      </c>
       <c r="S11" s="4"/>
       <c r="T11">
-        <f>SUM(B11:S11)</f>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:20" ht="18" x14ac:dyDescent="0.3">
@@ -887,17 +907,19 @@
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
+      <c r="E12" s="4">
+        <v>2</v>
+      </c>
       <c r="F12" s="4"/>
-      <c r="G12" s="4">
-        <v>1</v>
-      </c>
-      <c r="H12" s="4">
-        <v>2</v>
-      </c>
-      <c r="I12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4">
+        <v>3</v>
+      </c>
       <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
+      <c r="K12" s="4">
+        <v>1</v>
+      </c>
       <c r="L12" s="4"/>
       <c r="M12" s="4"/>
       <c r="N12" s="4"/>
@@ -907,8 +929,8 @@
       <c r="R12" s="4"/>
       <c r="S12" s="4"/>
       <c r="T12">
-        <f>SUM(B12:S12)</f>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:20" ht="18" x14ac:dyDescent="0.3">
@@ -920,57 +942,61 @@
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
-      <c r="G13" s="4">
-        <v>1</v>
-      </c>
-      <c r="H13" s="4">
-        <v>2</v>
-      </c>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
-      <c r="L13" s="4"/>
+      <c r="L13" s="4">
+        <v>3</v>
+      </c>
       <c r="M13" s="4"/>
-      <c r="N13" s="4"/>
-      <c r="O13" s="4"/>
+      <c r="N13" s="4">
+        <v>2</v>
+      </c>
+      <c r="O13" s="4">
+        <v>1</v>
+      </c>
       <c r="P13" s="4"/>
       <c r="Q13" s="4"/>
       <c r="R13" s="4"/>
       <c r="S13" s="4"/>
       <c r="T13">
-        <f>SUM(B13:S13)</f>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:20" ht="18" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="4"/>
+      <c r="B14" s="4">
+        <v>2</v>
+      </c>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
       <c r="H14" s="4">
-        <v>1</v>
-      </c>
-      <c r="I14" s="4">
-        <v>2</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="I14" s="4"/>
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
       <c r="L14" s="4"/>
       <c r="M14" s="4"/>
       <c r="N14" s="4"/>
       <c r="O14" s="4"/>
-      <c r="P14" s="4"/>
+      <c r="P14" s="4">
+        <v>1</v>
+      </c>
       <c r="Q14" s="4"/>
       <c r="R14" s="4"/>
       <c r="S14" s="4"/>
       <c r="T14">
-        <f>SUM(B14:S14)</f>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:20" ht="18" x14ac:dyDescent="0.3">
@@ -980,28 +1006,30 @@
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
+      <c r="E15" s="4">
+        <v>1</v>
+      </c>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
-      <c r="H15" s="4">
-        <v>1</v>
-      </c>
-      <c r="I15" s="4">
-        <v>2</v>
-      </c>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
       <c r="J15" s="4"/>
-      <c r="K15" s="4"/>
+      <c r="K15" s="4">
+        <v>2</v>
+      </c>
       <c r="L15" s="4"/>
       <c r="M15" s="4"/>
       <c r="N15" s="4"/>
-      <c r="O15" s="4"/>
+      <c r="O15" s="4">
+        <v>3</v>
+      </c>
       <c r="P15" s="4"/>
       <c r="Q15" s="4"/>
       <c r="R15" s="4"/>
       <c r="S15" s="4"/>
       <c r="T15">
-        <f>SUM(B15:S15)</f>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:20" ht="18" x14ac:dyDescent="0.3">
@@ -1009,15 +1037,15 @@
         <v>15</v>
       </c>
       <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
+      <c r="C16" s="4">
+        <v>1</v>
+      </c>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
-      <c r="I16" s="4">
-        <v>1</v>
-      </c>
+      <c r="I16" s="4"/>
       <c r="J16" s="4">
         <v>2</v>
       </c>
@@ -1026,13 +1054,15 @@
       <c r="M16" s="4"/>
       <c r="N16" s="4"/>
       <c r="O16" s="4"/>
-      <c r="P16" s="4"/>
+      <c r="P16" s="4">
+        <v>3</v>
+      </c>
       <c r="Q16" s="4"/>
       <c r="R16" s="4"/>
       <c r="S16" s="4"/>
       <c r="T16">
-        <f>SUM(B16:S16)</f>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:20" ht="18" x14ac:dyDescent="0.3">
@@ -1040,49 +1070,53 @@
         <v>16</v>
       </c>
       <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
+      <c r="C17" s="4">
+        <v>3</v>
+      </c>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4">
-        <v>1</v>
-      </c>
-      <c r="J17" s="4">
-        <v>2</v>
-      </c>
+      <c r="H17" s="4">
+        <v>1</v>
+      </c>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
       <c r="K17" s="4"/>
       <c r="L17" s="4"/>
       <c r="M17" s="4"/>
       <c r="N17" s="4"/>
       <c r="O17" s="4"/>
-      <c r="P17" s="4"/>
+      <c r="P17" s="4">
+        <v>2</v>
+      </c>
       <c r="Q17" s="4"/>
       <c r="R17" s="4"/>
       <c r="S17" s="4"/>
       <c r="T17">
-        <f>SUM(B17:S17)</f>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:20" ht="18" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="4"/>
+      <c r="B18" s="4">
+        <v>3</v>
+      </c>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
+      <c r="G18" s="4">
+        <v>2</v>
+      </c>
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
-      <c r="J18" s="4">
-        <v>1</v>
-      </c>
+      <c r="J18" s="4"/>
       <c r="K18" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L18" s="4"/>
       <c r="M18" s="4"/>
@@ -1093,8 +1127,8 @@
       <c r="R18" s="4"/>
       <c r="S18" s="4"/>
       <c r="T18">
-        <f>SUM(B18:S18)</f>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:20" ht="18" x14ac:dyDescent="0.3">
@@ -1109,23 +1143,25 @@
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
-      <c r="J19" s="4">
-        <v>1</v>
-      </c>
-      <c r="K19" s="4">
-        <v>2</v>
-      </c>
-      <c r="L19" s="4"/>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="4">
+        <v>3</v>
+      </c>
       <c r="M19" s="4"/>
-      <c r="N19" s="4"/>
-      <c r="O19" s="4"/>
+      <c r="N19" s="4">
+        <v>2</v>
+      </c>
+      <c r="O19" s="4">
+        <v>1</v>
+      </c>
       <c r="P19" s="4"/>
       <c r="Q19" s="4"/>
       <c r="R19" s="4"/>
       <c r="S19" s="4"/>
       <c r="T19">
-        <f>SUM(B19:S19)</f>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
     </row>
     <row r="20" spans="1:20" ht="18" x14ac:dyDescent="0.3">
@@ -1142,43 +1178,47 @@
       <c r="I20" s="4"/>
       <c r="J20" s="4"/>
       <c r="K20" s="4">
-        <v>1</v>
-      </c>
-      <c r="L20" s="4">
-        <v>2</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="L20" s="4"/>
       <c r="M20" s="4"/>
       <c r="N20" s="4"/>
-      <c r="O20" s="4"/>
+      <c r="O20" s="4">
+        <v>3</v>
+      </c>
       <c r="P20" s="4"/>
-      <c r="Q20" s="4"/>
+      <c r="Q20" s="4">
+        <v>1</v>
+      </c>
       <c r="R20" s="4"/>
       <c r="S20" s="4"/>
       <c r="T20">
-        <f>SUM(B20:S20)</f>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
     </row>
     <row r="21" spans="1:20" ht="18" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="4"/>
+      <c r="B21" s="4">
+        <v>2</v>
+      </c>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
+      <c r="F21" s="4">
+        <v>3</v>
+      </c>
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
       <c r="I21" s="4"/>
       <c r="J21" s="4"/>
-      <c r="K21" s="4">
-        <v>1</v>
-      </c>
-      <c r="L21" s="4">
-        <v>2</v>
-      </c>
-      <c r="M21" s="4"/>
+      <c r="K21" s="4"/>
+      <c r="L21" s="4"/>
+      <c r="M21" s="4">
+        <v>1</v>
+      </c>
       <c r="N21" s="4"/>
       <c r="O21" s="4"/>
       <c r="P21" s="4"/>
@@ -1186,8 +1226,8 @@
       <c r="R21" s="4"/>
       <c r="S21" s="4"/>
       <c r="T21">
-        <f>SUM(B21:S21)</f>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
     </row>
     <row r="22" spans="1:20" ht="18" x14ac:dyDescent="0.3">
@@ -1199,26 +1239,28 @@
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
+      <c r="G22" s="4">
+        <v>3</v>
+      </c>
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
-      <c r="J22" s="4"/>
+      <c r="J22" s="4">
+        <v>1</v>
+      </c>
       <c r="K22" s="4"/>
-      <c r="L22" s="4">
-        <v>1</v>
-      </c>
-      <c r="M22" s="4">
-        <v>2</v>
-      </c>
+      <c r="L22" s="4"/>
+      <c r="M22" s="4"/>
       <c r="N22" s="4"/>
       <c r="O22" s="4"/>
       <c r="P22" s="4"/>
       <c r="Q22" s="4"/>
       <c r="R22" s="4"/>
-      <c r="S22" s="4"/>
+      <c r="S22" s="4">
+        <v>2</v>
+      </c>
       <c r="T22">
-        <f>SUM(B22:S22)</f>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
     </row>
     <row r="23" spans="1:20" ht="18" x14ac:dyDescent="0.3">
@@ -1229,18 +1271,20 @@
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
+      <c r="F23" s="4">
+        <v>3</v>
+      </c>
+      <c r="G23" s="4">
+        <v>2</v>
+      </c>
       <c r="H23" s="4"/>
-      <c r="I23" s="4"/>
+      <c r="I23" s="4">
+        <v>1</v>
+      </c>
       <c r="J23" s="4"/>
       <c r="K23" s="4"/>
-      <c r="L23" s="4">
-        <v>1</v>
-      </c>
-      <c r="M23" s="4">
-        <v>2</v>
-      </c>
+      <c r="L23" s="4"/>
+      <c r="M23" s="4"/>
       <c r="N23" s="4"/>
       <c r="O23" s="4"/>
       <c r="P23" s="4"/>
@@ -1248,15 +1292,17 @@
       <c r="R23" s="4"/>
       <c r="S23" s="4"/>
       <c r="T23">
-        <f>SUM(B23:S23)</f>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
     </row>
     <row r="24" spans="1:20" ht="18" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B24" s="4"/>
+      <c r="B24" s="4">
+        <v>1</v>
+      </c>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
@@ -1266,52 +1312,54 @@
       <c r="I24" s="4"/>
       <c r="J24" s="4"/>
       <c r="K24" s="4"/>
-      <c r="L24" s="4"/>
-      <c r="M24" s="4">
-        <v>1</v>
-      </c>
-      <c r="N24" s="4">
-        <v>2</v>
-      </c>
+      <c r="L24" s="4">
+        <v>2</v>
+      </c>
+      <c r="M24" s="4"/>
+      <c r="N24" s="4"/>
       <c r="O24" s="4"/>
-      <c r="P24" s="4"/>
+      <c r="P24" s="4">
+        <v>3</v>
+      </c>
       <c r="Q24" s="4"/>
       <c r="R24" s="4"/>
       <c r="S24" s="4"/>
       <c r="T24">
-        <f>SUM(B24:S24)</f>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
     </row>
     <row r="25" spans="1:20" ht="18" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B25" s="4"/>
+      <c r="B25" s="4">
+        <v>1</v>
+      </c>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
+      <c r="E25" s="4">
+        <v>2</v>
+      </c>
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>
       <c r="I25" s="4"/>
       <c r="J25" s="4"/>
-      <c r="K25" s="4"/>
+      <c r="K25" s="4">
+        <v>3</v>
+      </c>
       <c r="L25" s="4"/>
-      <c r="M25" s="4">
-        <v>1</v>
-      </c>
-      <c r="N25" s="4">
-        <v>2</v>
-      </c>
+      <c r="M25" s="4"/>
+      <c r="N25" s="4"/>
       <c r="O25" s="4"/>
       <c r="P25" s="4"/>
       <c r="Q25" s="4"/>
       <c r="R25" s="4"/>
       <c r="S25" s="4"/>
       <c r="T25">
-        <f>SUM(B25:S25)</f>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
     </row>
     <row r="26" spans="1:20" ht="18" x14ac:dyDescent="0.3">
@@ -1324,36 +1372,42 @@
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
-      <c r="H26" s="4"/>
+      <c r="H26" s="4">
+        <v>1</v>
+      </c>
       <c r="I26" s="4"/>
       <c r="J26" s="4"/>
       <c r="K26" s="4"/>
       <c r="L26" s="4"/>
       <c r="M26" s="4"/>
-      <c r="N26" s="4">
-        <v>1</v>
-      </c>
+      <c r="N26" s="4"/>
       <c r="O26" s="4">
         <v>2</v>
       </c>
       <c r="P26" s="4"/>
       <c r="Q26" s="4"/>
       <c r="R26" s="4"/>
-      <c r="S26" s="4"/>
+      <c r="S26" s="4">
+        <v>3</v>
+      </c>
       <c r="T26">
-        <f>SUM(B26:S26)</f>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
     </row>
     <row r="27" spans="1:20" ht="18" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="4"/>
+      <c r="B27" s="4">
+        <v>3</v>
+      </c>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
+      <c r="F27" s="4">
+        <v>1</v>
+      </c>
       <c r="G27" s="4"/>
       <c r="H27" s="4"/>
       <c r="I27" s="4"/>
@@ -1362,49 +1416,49 @@
       <c r="L27" s="4"/>
       <c r="M27" s="4"/>
       <c r="N27" s="4">
-        <v>1</v>
-      </c>
-      <c r="O27" s="4">
-        <v>2</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="O27" s="4"/>
       <c r="P27" s="4"/>
       <c r="Q27" s="4"/>
       <c r="R27" s="4"/>
       <c r="S27" s="4"/>
       <c r="T27">
-        <f>SUM(B27:S27)</f>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
     </row>
     <row r="28" spans="1:20" ht="18" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="4"/>
+      <c r="B28" s="4">
+        <v>2</v>
+      </c>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
+      <c r="F28" s="4">
+        <v>3</v>
+      </c>
       <c r="G28" s="4"/>
       <c r="H28" s="4"/>
       <c r="I28" s="4"/>
       <c r="J28" s="4"/>
-      <c r="K28" s="4"/>
+      <c r="K28" s="4">
+        <v>1</v>
+      </c>
       <c r="L28" s="4"/>
       <c r="M28" s="4"/>
       <c r="N28" s="4"/>
-      <c r="O28" s="4">
-        <v>1</v>
-      </c>
-      <c r="P28" s="4">
-        <v>2</v>
-      </c>
+      <c r="O28" s="4"/>
+      <c r="P28" s="4"/>
       <c r="Q28" s="4"/>
       <c r="R28" s="4"/>
       <c r="S28" s="4"/>
       <c r="T28">
-        <f>SUM(B28:S28)</f>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
     </row>
     <row r="29" spans="1:20" ht="18" x14ac:dyDescent="0.3">
@@ -1414,12 +1468,16 @@
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
+      <c r="E29" s="4">
+        <v>3</v>
+      </c>
       <c r="F29" s="4"/>
       <c r="G29" s="4"/>
       <c r="H29" s="4"/>
       <c r="I29" s="4"/>
-      <c r="J29" s="4"/>
+      <c r="J29" s="4">
+        <v>2</v>
+      </c>
       <c r="K29" s="4"/>
       <c r="L29" s="4"/>
       <c r="M29" s="4"/>
@@ -1427,15 +1485,13 @@
       <c r="O29" s="4">
         <v>1</v>
       </c>
-      <c r="P29" s="4">
-        <v>2</v>
-      </c>
+      <c r="P29" s="4"/>
       <c r="Q29" s="4"/>
       <c r="R29" s="4"/>
       <c r="S29" s="4"/>
       <c r="T29">
-        <f>SUM(B29:S29)</f>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
     </row>
     <row r="30" spans="1:20" ht="18" x14ac:dyDescent="0.3">
@@ -1457,16 +1513,18 @@
       <c r="N30" s="4"/>
       <c r="O30" s="4"/>
       <c r="P30" s="4">
-        <v>1</v>
-      </c>
-      <c r="Q30" s="4">
-        <v>2</v>
-      </c>
-      <c r="R30" s="4"/>
-      <c r="S30" s="4"/>
+        <v>3</v>
+      </c>
+      <c r="Q30" s="4"/>
+      <c r="R30" s="4">
+        <v>2</v>
+      </c>
+      <c r="S30" s="4">
+        <v>1</v>
+      </c>
       <c r="T30">
-        <f>SUM(B30:S30)</f>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
     </row>
     <row r="31" spans="1:20" ht="18" x14ac:dyDescent="0.3">
@@ -1474,7 +1532,9 @@
         <v>30</v>
       </c>
       <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
+      <c r="C31" s="4">
+        <v>1</v>
+      </c>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
@@ -1486,18 +1546,18 @@
       <c r="L31" s="4"/>
       <c r="M31" s="4"/>
       <c r="N31" s="4"/>
-      <c r="O31" s="4"/>
-      <c r="P31" s="4">
-        <v>1</v>
-      </c>
-      <c r="Q31" s="4">
-        <v>2</v>
-      </c>
+      <c r="O31" s="4">
+        <v>2</v>
+      </c>
+      <c r="P31" s="4"/>
+      <c r="Q31" s="4"/>
       <c r="R31" s="4"/>
-      <c r="S31" s="4"/>
+      <c r="S31" s="4">
+        <v>3</v>
+      </c>
       <c r="T31">
-        <f>SUM(B31:S31)</f>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
     </row>
     <row r="32" spans="1:20" ht="18" x14ac:dyDescent="0.3">
@@ -1507,11 +1567,15 @@
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
+      <c r="E32" s="4">
+        <v>2</v>
+      </c>
       <c r="F32" s="4"/>
       <c r="G32" s="4"/>
       <c r="H32" s="4"/>
-      <c r="I32" s="4"/>
+      <c r="I32" s="4">
+        <v>3</v>
+      </c>
       <c r="J32" s="4"/>
       <c r="K32" s="4"/>
       <c r="L32" s="4"/>
@@ -1522,13 +1586,11 @@
       <c r="Q32" s="4">
         <v>1</v>
       </c>
-      <c r="R32" s="4">
-        <v>2</v>
-      </c>
+      <c r="R32" s="4"/>
       <c r="S32" s="4"/>
       <c r="T32">
-        <f>SUM(B32:S32)</f>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
     </row>
     <row r="33" spans="1:20" ht="18" x14ac:dyDescent="0.3">
@@ -1537,29 +1599,31 @@
       </c>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
-      <c r="D33" s="4"/>
+      <c r="D33" s="4">
+        <v>2</v>
+      </c>
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
       <c r="G33" s="4"/>
       <c r="H33" s="4"/>
       <c r="I33" s="4"/>
-      <c r="J33" s="4"/>
+      <c r="J33" s="4">
+        <v>3</v>
+      </c>
       <c r="K33" s="4"/>
       <c r="L33" s="4"/>
       <c r="M33" s="4"/>
-      <c r="N33" s="4"/>
+      <c r="N33" s="4">
+        <v>1</v>
+      </c>
       <c r="O33" s="4"/>
       <c r="P33" s="4"/>
-      <c r="Q33" s="4">
-        <v>1</v>
-      </c>
-      <c r="R33" s="4">
-        <v>2</v>
-      </c>
+      <c r="Q33" s="4"/>
+      <c r="R33" s="4"/>
       <c r="S33" s="4"/>
       <c r="T33">
-        <f>SUM(B33:S33)</f>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
     </row>
     <row r="34" spans="1:20" ht="18" x14ac:dyDescent="0.3">
@@ -1573,34 +1637,40 @@
       <c r="F34" s="4"/>
       <c r="G34" s="4"/>
       <c r="H34" s="4"/>
-      <c r="I34" s="4"/>
-      <c r="J34" s="4"/>
+      <c r="I34" s="4">
+        <v>3</v>
+      </c>
+      <c r="J34" s="4">
+        <v>2</v>
+      </c>
       <c r="K34" s="4"/>
       <c r="L34" s="4"/>
-      <c r="M34" s="4"/>
+      <c r="M34" s="4">
+        <v>1</v>
+      </c>
       <c r="N34" s="4"/>
       <c r="O34" s="4"/>
       <c r="P34" s="4"/>
       <c r="Q34" s="4"/>
-      <c r="R34" s="4">
-        <v>1</v>
-      </c>
-      <c r="S34" s="4">
-        <v>2</v>
-      </c>
+      <c r="R34" s="4"/>
+      <c r="S34" s="4"/>
       <c r="T34">
-        <f>SUM(B34:S34)</f>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
     </row>
     <row r="35" spans="1:20" ht="18" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B35" s="4"/>
+      <c r="B35" s="4">
+        <v>3</v>
+      </c>
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>
-      <c r="E35" s="4"/>
+      <c r="E35" s="4">
+        <v>1</v>
+      </c>
       <c r="F35" s="4"/>
       <c r="G35" s="4"/>
       <c r="H35" s="4"/>
@@ -1611,17 +1681,15 @@
       <c r="M35" s="4"/>
       <c r="N35" s="4"/>
       <c r="O35" s="4"/>
-      <c r="P35" s="4"/>
+      <c r="P35" s="4">
+        <v>2</v>
+      </c>
       <c r="Q35" s="4"/>
-      <c r="R35" s="4">
-        <v>1</v>
-      </c>
-      <c r="S35" s="4">
-        <v>2</v>
-      </c>
+      <c r="R35" s="4"/>
+      <c r="S35" s="4"/>
       <c r="T35">
-        <f>SUM(B35:S35)</f>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
     </row>
     <row r="36" spans="1:20" ht="18" x14ac:dyDescent="0.3">
@@ -1632,42 +1700,50 @@
       <c r="C36" s="4"/>
       <c r="D36" s="4"/>
       <c r="E36" s="4"/>
-      <c r="F36" s="4"/>
+      <c r="F36" s="4">
+        <v>3</v>
+      </c>
       <c r="G36" s="4"/>
       <c r="H36" s="4"/>
       <c r="I36" s="4"/>
-      <c r="J36" s="4"/>
+      <c r="J36" s="4">
+        <v>2</v>
+      </c>
       <c r="K36" s="4"/>
       <c r="L36" s="4"/>
       <c r="M36" s="4"/>
       <c r="N36" s="4"/>
-      <c r="O36" s="4"/>
+      <c r="O36" s="4">
+        <v>1</v>
+      </c>
       <c r="P36" s="4"/>
       <c r="Q36" s="4"/>
-      <c r="R36" s="4">
-        <v>2</v>
-      </c>
-      <c r="S36" s="4">
-        <v>1</v>
-      </c>
+      <c r="R36" s="4"/>
+      <c r="S36" s="4"/>
       <c r="T36">
-        <f>SUM(B36:S36)</f>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
     </row>
     <row r="37" spans="1:20" ht="18" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B37" s="4"/>
+      <c r="B37" s="4">
+        <v>3</v>
+      </c>
       <c r="C37" s="4"/>
       <c r="D37" s="4"/>
       <c r="E37" s="4"/>
       <c r="F37" s="4"/>
-      <c r="G37" s="4"/>
+      <c r="G37" s="4">
+        <v>2</v>
+      </c>
       <c r="H37" s="4"/>
       <c r="I37" s="4"/>
-      <c r="J37" s="4"/>
+      <c r="J37" s="4">
+        <v>1</v>
+      </c>
       <c r="K37" s="4"/>
       <c r="L37" s="4"/>
       <c r="M37" s="4"/>
@@ -1675,89 +1751,85 @@
       <c r="O37" s="4"/>
       <c r="P37" s="4"/>
       <c r="Q37" s="4"/>
-      <c r="R37" s="4">
-        <v>2</v>
-      </c>
-      <c r="S37" s="4">
-        <v>1</v>
-      </c>
+      <c r="R37" s="4"/>
+      <c r="S37" s="4"/>
       <c r="T37">
-        <f>SUM(B37:S37)</f>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B38">
         <f>SUM(B2:B37)</f>
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="C38">
-        <f t="shared" ref="C38:S38" si="0">SUM(C2:C37)</f>
+        <f t="shared" ref="C38:S38" si="1">SUM(C2:C37)</f>
         <v>6</v>
       </c>
       <c r="D38">
-        <f t="shared" si="0"/>
-        <v>6</v>
+        <f t="shared" si="1"/>
+        <v>7</v>
       </c>
       <c r="E38">
-        <f t="shared" si="0"/>
-        <v>6</v>
+        <f t="shared" si="1"/>
+        <v>14</v>
       </c>
       <c r="F38">
-        <f t="shared" si="0"/>
-        <v>6</v>
+        <f t="shared" si="1"/>
+        <v>14</v>
       </c>
       <c r="G38">
-        <f t="shared" si="0"/>
-        <v>6</v>
+        <f t="shared" si="1"/>
+        <v>11</v>
       </c>
       <c r="H38">
-        <f t="shared" si="0"/>
-        <v>6</v>
+        <f t="shared" si="1"/>
+        <v>12</v>
       </c>
       <c r="I38">
-        <f t="shared" si="0"/>
-        <v>6</v>
+        <f t="shared" si="1"/>
+        <v>15</v>
       </c>
       <c r="J38">
-        <f t="shared" si="0"/>
-        <v>6</v>
+        <f t="shared" si="1"/>
+        <v>14</v>
       </c>
       <c r="K38">
-        <f t="shared" si="0"/>
-        <v>6</v>
+        <f t="shared" si="1"/>
+        <v>17</v>
       </c>
       <c r="L38">
-        <f t="shared" si="0"/>
-        <v>6</v>
+        <f t="shared" si="1"/>
+        <v>11</v>
       </c>
       <c r="M38">
-        <f t="shared" si="0"/>
-        <v>6</v>
+        <f t="shared" si="1"/>
+        <v>2</v>
       </c>
       <c r="N38">
-        <f t="shared" si="0"/>
-        <v>6</v>
+        <f t="shared" si="1"/>
+        <v>8</v>
       </c>
       <c r="O38">
-        <f t="shared" si="0"/>
-        <v>6</v>
+        <f t="shared" si="1"/>
+        <v>20</v>
       </c>
       <c r="P38">
-        <f t="shared" si="0"/>
-        <v>6</v>
+        <f t="shared" si="1"/>
+        <v>21</v>
       </c>
       <c r="Q38">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="R38">
-        <f t="shared" si="0"/>
-        <v>10</v>
+        <f t="shared" si="1"/>
+        <v>3</v>
       </c>
       <c r="S38">
-        <f t="shared" si="0"/>
-        <v>6</v>
+        <f t="shared" si="1"/>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Main avec verif tableau
</commit_message>
<xml_diff>
--- a/sujets choisis test.xlsx
+++ b/sujets choisis test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robin\OneDrive\Documents\Projet IESE4 - Allocation de ressources\AllocationDeRessource\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9E4F6F4-F470-4719-9C9C-1836EF76B5E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B14B7352-D269-42B3-B38B-A7C9505C474E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -501,8 +501,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="67" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="P27" sqref="P27"/>
+    <sheetView tabSelected="1" zoomScale="67" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>